<commit_message>
Contacts by age, infection status, daycare attendance
</commit_message>
<xml_diff>
--- a/My model/Baseline distribution.xlsx
+++ b/My model/Baseline distribution.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lshtm-my.sharepoint.com/personal/lsh2100076_student_lshtm_ac_uk/Documents/Documents/LSHTM/Project/My model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lshtm-my.sharepoint.com/personal/lsh2100076_student_lshtm_ac_uk/Documents/Documents/LSHTM/Project/RSV_infection_NL/My model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="10_ncr:40000_{29F300FD-C409-4E60-8CB2-F1B321ADD497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5463ACF3-71FD-4B54-9DAB-C4EB3494CE46}"/>
+  <xr:revisionPtr revIDLastSave="711" documentId="10_ncr:40000_{29F300FD-C409-4E60-8CB2-F1B321ADD497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D11193B7-6F75-400F-9F50-0EBA9903BBB8}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="Contacts 0-4" sheetId="14" r:id="rId12"/>
     <sheet name="Contacts 5-9" sheetId="15" r:id="rId13"/>
     <sheet name="RSV infection" sheetId="16" r:id="rId14"/>
+    <sheet name="Contacts by age" sheetId="17" r:id="rId15"/>
+    <sheet name="Contacts by age and nursery" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="66">
   <si>
     <t>Variable</t>
   </si>
@@ -186,6 +188,66 @@
   </si>
   <si>
     <t>RSV infection</t>
+  </si>
+  <si>
+    <t>Total contacts by age group</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>0-1 year</t>
+  </si>
+  <si>
+    <t>2-3 years</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>Total contact by age group among infected children</t>
+  </si>
+  <si>
+    <t>Total contact by age group among uninfected children</t>
+  </si>
+  <si>
+    <t>Contacts aged 0-4 years by age group</t>
+  </si>
+  <si>
+    <t>Contacts aged 0-4 years by age group among infected children</t>
+  </si>
+  <si>
+    <t>Contacts aged 0-4 years by age group among uninfected children</t>
+  </si>
+  <si>
+    <t>Contacts aged 5-9 years by age group</t>
+  </si>
+  <si>
+    <t>Contacts aged 5-9 years by age group among infected children</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Total contact by age group among infected children who went to day care</t>
+  </si>
+  <si>
+    <t>Total contact by age group among infected children who didn't go to daycare</t>
+  </si>
+  <si>
+    <t>Total contact by age group among uninfected children who didn't go to daycare</t>
+  </si>
+  <si>
+    <t>Total contact by age group among uninfected children who went to day care</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -11370,7 +11432,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{DAF336FC-264F-4F5B-8210-2BA3E9587F05}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11381,7 +11443,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1C63F5AC-F205-42FB-B92C-7626921A207B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11425,7 +11487,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{28A44A8F-DE3C-4989-925D-BDB3785AC43C}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11469,7 +11531,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6D4EDBE9-7A4E-4633-9695-82F81F0C6FB6}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11513,7 +11575,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8660230" cy="6285247"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11546,7 +11608,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8660230" cy="6285247"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11678,7 +11740,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8656236" cy="6285453"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11810,7 +11872,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8660230" cy="6285247"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -14412,4 +14474,1363 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B866F7E-6D44-4413-9BA9-AC165AF961BC}">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>5.24</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>6.52</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.7991967871485901</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3.62782695073866</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.28514056199999999</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.82977605799999998</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8.25</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>14.29</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2.5867768595041301</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3.9405359650001999</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.72727272700000001</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1.6733200530000001</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>11.32</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4.3035714285714297</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K5" s="2">
+        <v>6.3615882603957603</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1.553571429</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2">
+        <v>3.050601388</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>17.09</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>28.47</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5.9565217391304301</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.8862391662701103</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>30</v>
+      </c>
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2.8043478259999999</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="R6" s="2">
+        <v>5.4021377050000003</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>23.37</v>
+      </c>
+      <c r="C7">
+        <v>22.5</v>
+      </c>
+      <c r="D7">
+        <v>19.64</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2">
+        <v>9.0625</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+      <c r="K7" s="2">
+        <v>10.2514751102212</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>40</v>
+      </c>
+      <c r="O7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="2">
+        <v>7.375</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>3</v>
+      </c>
+      <c r="R7" s="2">
+        <v>11.215628499999999</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>6.02</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>6.32</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11">
+        <v>2.57</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+      <c r="O11" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0.28514056199999999</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.82977605799999998</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>16.59</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>3.33</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K12">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>20</v>
+      </c>
+      <c r="O12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1.78</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>11.53</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13">
+        <v>4.51</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>6.47</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.58</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>17.09</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>28.47</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>200</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>5.96</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K14" s="2">
+        <v>6.8862391662701103</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="O14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="2">
+        <v>2.8043478259999999</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="2">
+        <v>5.4021377050000003</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>23.37</v>
+      </c>
+      <c r="C15">
+        <v>22.5</v>
+      </c>
+      <c r="D15">
+        <v>19.64</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>82</v>
+      </c>
+      <c r="H15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15">
+        <v>0.06</v>
+      </c>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2">
+        <v>10.2514751102212</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>40</v>
+      </c>
+      <c r="O15" t="s">
+        <v>51</v>
+      </c>
+      <c r="P15" s="2">
+        <v>7.375</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3</v>
+      </c>
+      <c r="R15" s="2">
+        <v>11.215628499999999</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R18" t="s">
+        <v>48</v>
+      </c>
+      <c r="S18" t="s">
+        <v>59</v>
+      </c>
+      <c r="T18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>5.03</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>6.57</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>71</v>
+      </c>
+      <c r="H19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19">
+        <v>1.57</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>3.23</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>27</v>
+      </c>
+      <c r="O19" t="s">
+        <v>49</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>5.59</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>0.89</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1.73</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>10</v>
+      </c>
+      <c r="O20" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1.42</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>5.33</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>3.05</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21">
+        <v>0.66</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="O21" t="s">
+        <v>50</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0362B99-1845-46ED-AAEB-DCC2C820AF99}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.53</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7.54</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="2">
+        <v>6.28</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5.01</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10.19</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8.11</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2.86</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>3.18</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5</v>
+      </c>
+      <c r="L5" s="2">
+        <v>4.24</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>17.93</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30.27</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>25.21</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.09</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="2">
+        <v>4.67</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4</v>
+      </c>
+      <c r="L11" s="2">
+        <v>7.1970000000000001</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8.32</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>22.2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="I12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="2">
+        <v>6</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4.9598000000000004</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>16.32</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>76</v>
+      </c>
+      <c r="I13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="2">
+        <v>6</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12.67</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>11.04</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2">
+        <v>21.21</v>
+      </c>
+      <c r="C15" s="2">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2">
+        <v>16.04</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>